<commit_message>
Physics mock framework setup
</commit_message>
<xml_diff>
--- a/Mathematics/Analysis.xlsx
+++ b/Mathematics/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeep/Documents/StudyNotes/ICSE-X-MockTests/Mathematics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8F32F3-8EBF-4F44-A63C-9F05ABE0BA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACFCB2C-9D3C-C44E-A181-F34283E946F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" xr2:uid="{B4465AD6-530F-2F46-9D03-3D425B2D33AA}"/>
   </bookViews>
@@ -677,16 +677,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -814,6 +814,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:val>
             <c:numRef>
               <c:f>(Sheet1!$F$28,Sheet1!$H$28,Sheet1!$J$28,Sheet1!$L$28,Sheet1!$N$28,Sheet1!$P$28,Sheet1!$R$28,Sheet1!$T$28,Sheet1!$V$28,Sheet1!$X$28,Sheet1!$Z$28,Sheet1!$AB$28,Sheet1!$AD$28,Sheet1!$AF$28,Sheet1!$AH$28,Sheet1!$AJ$28)</c:f>
@@ -851,19 +865,19 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1609,13 +1623,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>42333</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>194733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>177799</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>33866</xdr:rowOff>
     </xdr:to>
@@ -1944,9 +1958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FA7AF1-E407-A940-8659-99844D0177BA}">
   <dimension ref="A1:AM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2006,16 +2020,24 @@
       </c>
       <c r="X1" s="51"/>
       <c r="Y1" s="50">
-        <v>45423</v>
+        <v>45424</v>
       </c>
       <c r="Z1" s="51"/>
-      <c r="AA1" s="50"/>
+      <c r="AA1" s="50">
+        <v>45431</v>
+      </c>
       <c r="AB1" s="51"/>
-      <c r="AC1" s="50"/>
+      <c r="AC1" s="50">
+        <v>45434</v>
+      </c>
       <c r="AD1" s="51"/>
-      <c r="AE1" s="50"/>
+      <c r="AE1" s="50">
+        <v>45437</v>
+      </c>
       <c r="AF1" s="51"/>
-      <c r="AG1" s="50"/>
+      <c r="AG1" s="50">
+        <v>45442</v>
+      </c>
       <c r="AH1" s="51"/>
       <c r="AI1" s="50"/>
       <c r="AJ1" s="51"/>
@@ -2253,15 +2275,15 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5:B27" si="0">SUM(E5,G5,I5,K5,M5,O5,Q5,S5,U5,W5,Y5,AA5,AC5,AE5,AG5,AI5)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C27" si="1">SUM(F5,H5,J5,L5,N5,P5,R5,T5,V5,X5,Z5,AB5,AD5,AF5,AH5,AJ5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="25">
         <f t="shared" ref="D5:D27" si="2">IF(B5=0,0,((B5-C5)/B5)*100)</f>
-        <v>92.307692307692307</v>
+        <v>89.473684210526315</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="8"/>
@@ -2299,17 +2321,27 @@
         <v>1</v>
       </c>
       <c r="X5" s="8"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="8"/>
+      <c r="Y5" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>1</v>
+      </c>
       <c r="AA5" s="16"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="8"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="16"/>
+      <c r="AE5" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="16">
+        <v>1</v>
+      </c>
       <c r="AH5" s="8"/>
-      <c r="AI5" s="16"/>
+      <c r="AI5" s="16">
+        <v>2</v>
+      </c>
       <c r="AJ5" s="8"/>
     </row>
     <row r="6" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
@@ -2355,7 +2387,7 @@
       <c r="AC6" s="16"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="16"/>
-      <c r="AF6" s="8"/>
+      <c r="AF6" s="35"/>
       <c r="AG6" s="16"/>
       <c r="AH6" s="8"/>
       <c r="AI6" s="16"/>
@@ -2367,7 +2399,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
@@ -2375,7 +2407,7 @@
       </c>
       <c r="D7" s="25">
         <f t="shared" si="2"/>
-        <v>82.35294117647058</v>
+        <v>85.714285714285708</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="8"/>
@@ -2419,15 +2451,21 @@
       <c r="V7" s="35"/>
       <c r="W7" s="16"/>
       <c r="X7" s="8"/>
-      <c r="Y7" s="16"/>
+      <c r="Y7" s="16">
+        <v>1</v>
+      </c>
       <c r="Z7" s="8"/>
       <c r="AA7" s="16"/>
       <c r="AB7" s="8"/>
       <c r="AC7" s="16"/>
       <c r="AD7" s="8"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="16"/>
+      <c r="AE7" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="16">
+        <v>1</v>
+      </c>
       <c r="AH7" s="8"/>
       <c r="AI7" s="16"/>
       <c r="AJ7" s="8"/>
@@ -2438,15 +2476,15 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="25">
         <f t="shared" si="2"/>
-        <v>80.952380952380949</v>
+        <v>84.848484848484844</v>
       </c>
       <c r="E8" s="16">
         <v>4</v>
@@ -2496,17 +2534,31 @@
       <c r="X8" s="8">
         <v>1</v>
       </c>
-      <c r="Y8" s="16"/>
+      <c r="Y8" s="16">
+        <v>3</v>
+      </c>
       <c r="Z8" s="8"/>
-      <c r="AA8" s="16"/>
+      <c r="AA8" s="16">
+        <v>1</v>
+      </c>
       <c r="AB8" s="8"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="16"/>
+      <c r="AC8" s="16">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="16">
+        <v>2</v>
+      </c>
       <c r="AH8" s="8"/>
-      <c r="AI8" s="16"/>
+      <c r="AI8" s="16">
+        <v>1</v>
+      </c>
       <c r="AJ8" s="8"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
@@ -2515,7 +2567,7 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -2559,15 +2611,23 @@
         <v>2</v>
       </c>
       <c r="X9" s="8"/>
-      <c r="Y9" s="16"/>
+      <c r="Y9" s="16">
+        <v>1</v>
+      </c>
       <c r="Z9" s="8"/>
       <c r="AA9" s="16"/>
       <c r="AB9" s="8"/>
-      <c r="AC9" s="16"/>
+      <c r="AC9" s="16">
+        <v>2</v>
+      </c>
       <c r="AD9" s="8"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="16"/>
+      <c r="AE9" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="16">
+        <v>2</v>
+      </c>
       <c r="AH9" s="8"/>
       <c r="AI9" s="16"/>
       <c r="AJ9" s="8"/>
@@ -2578,7 +2638,7 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
@@ -2586,7 +2646,7 @@
       </c>
       <c r="D10" s="25">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>89.65517241379311</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="8"/>
@@ -2630,15 +2690,25 @@
         <v>2</v>
       </c>
       <c r="X10" s="8"/>
-      <c r="Y10" s="16"/>
+      <c r="Y10" s="16">
+        <v>1</v>
+      </c>
       <c r="Z10" s="8"/>
-      <c r="AA10" s="16"/>
+      <c r="AA10" s="16">
+        <v>5</v>
+      </c>
       <c r="AB10" s="8"/>
-      <c r="AC10" s="16"/>
+      <c r="AC10" s="16">
+        <v>1</v>
+      </c>
       <c r="AD10" s="8"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="16"/>
+      <c r="AE10" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="16">
+        <v>1</v>
+      </c>
       <c r="AH10" s="8"/>
       <c r="AI10" s="16"/>
       <c r="AJ10" s="8"/>
@@ -2649,7 +2719,7 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
@@ -2657,7 +2727,7 @@
       </c>
       <c r="D11" s="25">
         <f t="shared" si="2"/>
-        <v>77.272727272727266</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="E11" s="16">
         <v>3</v>
@@ -2709,15 +2779,25 @@
       <c r="X11" s="8">
         <v>1</v>
       </c>
-      <c r="Y11" s="16"/>
+      <c r="Y11" s="16">
+        <v>1</v>
+      </c>
       <c r="Z11" s="8"/>
-      <c r="AA11" s="16"/>
+      <c r="AA11" s="16">
+        <v>1</v>
+      </c>
       <c r="AB11" s="8"/>
-      <c r="AC11" s="16"/>
+      <c r="AC11" s="16">
+        <v>2</v>
+      </c>
       <c r="AD11" s="8"/>
-      <c r="AE11" s="16"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="16"/>
+      <c r="AE11" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="35"/>
+      <c r="AG11" s="16">
+        <v>2</v>
+      </c>
       <c r="AH11" s="8"/>
       <c r="AI11" s="16"/>
       <c r="AJ11" s="8"/>
@@ -2728,15 +2808,15 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="25">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="8"/>
@@ -2760,26 +2840,40 @@
         <v>2</v>
       </c>
       <c r="X12" s="8"/>
-      <c r="Y12" s="16"/>
+      <c r="Y12" s="16">
+        <v>2</v>
+      </c>
       <c r="Z12" s="8"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="16"/>
+      <c r="AA12" s="16">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="16">
+        <v>2</v>
+      </c>
       <c r="AD12" s="8"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="8"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="8"/>
+      <c r="AE12" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="16">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="8">
+        <v>1</v>
+      </c>
       <c r="AI12" s="16"/>
       <c r="AJ12" s="8"/>
     </row>
-    <row r="13" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="1"/>
@@ -2787,7 +2881,7 @@
       </c>
       <c r="D13" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="8"/>
@@ -2816,8 +2910,10 @@
       <c r="AC13" s="16"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="16"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="16"/>
+      <c r="AF13" s="35"/>
+      <c r="AG13" s="16">
+        <v>1</v>
+      </c>
       <c r="AH13" s="8"/>
       <c r="AI13" s="16"/>
       <c r="AJ13" s="8"/>
@@ -2865,7 +2961,7 @@
       <c r="AC14" s="16"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="16"/>
-      <c r="AF14" s="8"/>
+      <c r="AF14" s="35"/>
       <c r="AG14" s="16"/>
       <c r="AH14" s="8"/>
       <c r="AI14" s="16"/>
@@ -2914,7 +3010,7 @@
       <c r="AC15" s="16"/>
       <c r="AD15" s="8"/>
       <c r="AE15" s="16"/>
-      <c r="AF15" s="8"/>
+      <c r="AF15" s="35"/>
       <c r="AG15" s="16"/>
       <c r="AH15" s="8"/>
       <c r="AI15" s="16"/>
@@ -2963,7 +3059,7 @@
       <c r="AC16" s="16"/>
       <c r="AD16" s="8"/>
       <c r="AE16" s="16"/>
-      <c r="AF16" s="8"/>
+      <c r="AF16" s="35"/>
       <c r="AG16" s="16"/>
       <c r="AH16" s="8"/>
       <c r="AI16" s="16"/>
@@ -3012,7 +3108,7 @@
       <c r="AC17" s="16"/>
       <c r="AD17" s="8"/>
       <c r="AE17" s="16"/>
-      <c r="AF17" s="8"/>
+      <c r="AF17" s="35"/>
       <c r="AG17" s="16"/>
       <c r="AH17" s="8"/>
       <c r="AI17" s="16"/>
@@ -3061,7 +3157,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="8"/>
       <c r="AE18" s="16"/>
-      <c r="AF18" s="8"/>
+      <c r="AF18" s="35"/>
       <c r="AG18" s="16"/>
       <c r="AH18" s="8"/>
       <c r="AI18" s="16"/>
@@ -3110,7 +3206,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="8"/>
       <c r="AE19" s="16"/>
-      <c r="AF19" s="8"/>
+      <c r="AF19" s="35"/>
       <c r="AG19" s="16"/>
       <c r="AH19" s="8"/>
       <c r="AI19" s="16"/>
@@ -3159,7 +3255,7 @@
       <c r="AC20" s="16"/>
       <c r="AD20" s="8"/>
       <c r="AE20" s="16"/>
-      <c r="AF20" s="8"/>
+      <c r="AF20" s="35"/>
       <c r="AG20" s="16"/>
       <c r="AH20" s="8"/>
       <c r="AI20" s="16"/>
@@ -3208,19 +3304,19 @@
       <c r="AC21" s="16"/>
       <c r="AD21" s="8"/>
       <c r="AE21" s="16"/>
-      <c r="AF21" s="8"/>
+      <c r="AF21" s="35"/>
       <c r="AG21" s="16"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="16"/>
       <c r="AJ21" s="8"/>
     </row>
-    <row r="22" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="1"/>
@@ -3228,7 +3324,7 @@
       </c>
       <c r="D22" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="8"/>
@@ -3254,11 +3350,17 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="16"/>
       <c r="AB22" s="8"/>
-      <c r="AC22" s="16"/>
+      <c r="AC22" s="16">
+        <v>1</v>
+      </c>
       <c r="AD22" s="8"/>
-      <c r="AE22" s="16"/>
-      <c r="AF22" s="8"/>
-      <c r="AG22" s="16"/>
+      <c r="AE22" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF22" s="35"/>
+      <c r="AG22" s="16">
+        <v>2</v>
+      </c>
       <c r="AH22" s="8"/>
       <c r="AI22" s="16"/>
       <c r="AJ22" s="8"/>
@@ -3269,7 +3371,7 @@
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="1"/>
@@ -3277,7 +3379,7 @@
       </c>
       <c r="D23" s="25">
         <f t="shared" si="2"/>
-        <v>85.714285714285708</v>
+        <v>90</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="8"/>
@@ -3321,15 +3423,25 @@
         <v>3</v>
       </c>
       <c r="X23" s="8"/>
-      <c r="Y23" s="16"/>
+      <c r="Y23" s="16">
+        <v>2</v>
+      </c>
       <c r="Z23" s="8"/>
-      <c r="AA23" s="16"/>
+      <c r="AA23" s="16">
+        <v>2</v>
+      </c>
       <c r="AB23" s="8"/>
-      <c r="AC23" s="16"/>
+      <c r="AC23" s="16">
+        <v>2</v>
+      </c>
       <c r="AD23" s="8"/>
-      <c r="AE23" s="16"/>
-      <c r="AF23" s="8"/>
-      <c r="AG23" s="16"/>
+      <c r="AE23" s="16">
+        <v>2</v>
+      </c>
+      <c r="AF23" s="35"/>
+      <c r="AG23" s="16">
+        <v>1</v>
+      </c>
       <c r="AH23" s="8"/>
       <c r="AI23" s="16"/>
       <c r="AJ23" s="8"/>
@@ -3340,7 +3452,7 @@
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="1"/>
@@ -3374,14 +3486,22 @@
       <c r="V24" s="35"/>
       <c r="W24" s="16"/>
       <c r="X24" s="8"/>
-      <c r="Y24" s="16"/>
+      <c r="Y24" s="16">
+        <v>1</v>
+      </c>
       <c r="Z24" s="8"/>
-      <c r="AA24" s="16"/>
+      <c r="AA24" s="16">
+        <v>1</v>
+      </c>
       <c r="AB24" s="8"/>
-      <c r="AC24" s="16"/>
+      <c r="AC24" s="16">
+        <v>1</v>
+      </c>
       <c r="AD24" s="8"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="8"/>
+      <c r="AE24" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="35"/>
       <c r="AG24" s="16"/>
       <c r="AH24" s="8"/>
       <c r="AI24" s="16"/>
@@ -3430,7 +3550,7 @@
       <c r="AC25" s="16"/>
       <c r="AD25" s="8"/>
       <c r="AE25" s="16"/>
-      <c r="AF25" s="8"/>
+      <c r="AF25" s="35"/>
       <c r="AG25" s="16"/>
       <c r="AH25" s="8"/>
       <c r="AI25" s="16"/>
@@ -3442,7 +3562,7 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="1"/>
@@ -3450,7 +3570,7 @@
       </c>
       <c r="D26" s="25">
         <f t="shared" si="2"/>
-        <v>87.5</v>
+        <v>90.476190476190482</v>
       </c>
       <c r="E26" s="16">
         <v>2</v>
@@ -3494,15 +3614,23 @@
         <v>1</v>
       </c>
       <c r="X26" s="8"/>
-      <c r="Y26" s="16"/>
+      <c r="Y26" s="16">
+        <v>1</v>
+      </c>
       <c r="Z26" s="8"/>
-      <c r="AA26" s="16"/>
+      <c r="AA26" s="16">
+        <v>2</v>
+      </c>
       <c r="AB26" s="8"/>
-      <c r="AC26" s="16"/>
+      <c r="AC26" s="16">
+        <v>1</v>
+      </c>
       <c r="AD26" s="8"/>
       <c r="AE26" s="16"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="16"/>
+      <c r="AF26" s="35"/>
+      <c r="AG26" s="16">
+        <v>1</v>
+      </c>
       <c r="AH26" s="8"/>
       <c r="AI26" s="16"/>
       <c r="AJ26" s="8"/>
@@ -3562,15 +3690,15 @@
       </c>
       <c r="B28" s="20">
         <f>SUM(B4:B27)</f>
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="C28" s="20">
         <f>SUM(C4:C27)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D28" s="24">
         <f>((B28-C28)/B28)*100</f>
-        <v>85.61643835616438</v>
+        <v>88.888888888888886</v>
       </c>
       <c r="E28" s="21">
         <f>SUM(E4:E27)</f>
@@ -3654,31 +3782,31 @@
       </c>
       <c r="Y28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Z28" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB28" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD28" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AF28" s="22">
         <f t="shared" si="3"/>
@@ -3686,15 +3814,15 @@
       </c>
       <c r="AG28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AH28" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ28" s="22">
         <f t="shared" si="3"/>
@@ -3708,50 +3836,52 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6">
         <f>SUM(E31:AJ31)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D31" s="29">
         <f>C31/$C$28</f>
-        <v>0.23809523809523808</v>
-      </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="46">
-        <v>1</v>
-      </c>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="46">
-        <v>2</v>
-      </c>
-      <c r="R31" s="47"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="49"/>
-      <c r="W31" s="46">
-        <v>2</v>
-      </c>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="46"/>
-      <c r="Z31" s="47"/>
-      <c r="AA31" s="46"/>
-      <c r="AB31" s="47"/>
-      <c r="AC31" s="46"/>
-      <c r="AD31" s="47"/>
+        <v>0.24</v>
+      </c>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="48">
+        <v>1</v>
+      </c>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="48">
+        <v>2</v>
+      </c>
+      <c r="R31" s="49"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="46"/>
+      <c r="V31" s="47"/>
+      <c r="W31" s="48">
+        <v>2</v>
+      </c>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="49"/>
+      <c r="AA31" s="48">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="49"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="49"/>
       <c r="AE31" s="46"/>
       <c r="AF31" s="47"/>
-      <c r="AG31" s="46"/>
-      <c r="AH31" s="47"/>
-      <c r="AI31" s="46"/>
-      <c r="AJ31" s="47"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="49"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="49"/>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
@@ -3764,7 +3894,7 @@
       </c>
       <c r="D32" s="30">
         <f t="shared" ref="D32:D42" si="5">C32/$C$28</f>
-        <v>4.7619047619047616E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="41"/>
@@ -3794,8 +3924,8 @@
       <c r="AB32" s="41"/>
       <c r="AC32" s="40"/>
       <c r="AD32" s="41"/>
-      <c r="AE32" s="40"/>
-      <c r="AF32" s="41"/>
+      <c r="AE32" s="42"/>
+      <c r="AF32" s="43"/>
       <c r="AG32" s="40"/>
       <c r="AH32" s="41"/>
       <c r="AI32" s="40"/>
@@ -3840,8 +3970,8 @@
       <c r="AB33" s="41"/>
       <c r="AC33" s="40"/>
       <c r="AD33" s="41"/>
-      <c r="AE33" s="40"/>
-      <c r="AF33" s="41"/>
+      <c r="AE33" s="42"/>
+      <c r="AF33" s="43"/>
       <c r="AG33" s="40"/>
       <c r="AH33" s="41"/>
       <c r="AI33" s="40"/>
@@ -3854,11 +3984,11 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2">
         <f>SUM(E34:AJ34)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="30">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
+        <v>0.16</v>
       </c>
       <c r="E34" s="40">
         <v>1</v>
@@ -3886,14 +4016,16 @@
       <c r="V34" s="43"/>
       <c r="W34" s="40"/>
       <c r="X34" s="41"/>
-      <c r="Y34" s="40"/>
+      <c r="Y34" s="40">
+        <v>1</v>
+      </c>
       <c r="Z34" s="41"/>
       <c r="AA34" s="40"/>
       <c r="AB34" s="41"/>
       <c r="AC34" s="40"/>
       <c r="AD34" s="41"/>
-      <c r="AE34" s="40"/>
-      <c r="AF34" s="41"/>
+      <c r="AE34" s="42"/>
+      <c r="AF34" s="43"/>
       <c r="AG34" s="40"/>
       <c r="AH34" s="41"/>
       <c r="AI34" s="40"/>
@@ -3906,11 +4038,11 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" s="30">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
+        <v>0.16</v>
       </c>
       <c r="E35" s="40"/>
       <c r="F35" s="41"/>
@@ -3940,10 +4072,12 @@
       <c r="Z35" s="41"/>
       <c r="AA35" s="40"/>
       <c r="AB35" s="41"/>
-      <c r="AC35" s="40"/>
+      <c r="AC35" s="40">
+        <v>1</v>
+      </c>
       <c r="AD35" s="41"/>
-      <c r="AE35" s="40"/>
-      <c r="AF35" s="41"/>
+      <c r="AE35" s="42"/>
+      <c r="AF35" s="43"/>
       <c r="AG35" s="40"/>
       <c r="AH35" s="41"/>
       <c r="AI35" s="40"/>
@@ -3956,11 +4090,11 @@
       <c r="B36" s="28"/>
       <c r="C36" s="28">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D36" s="31">
         <f t="shared" si="5"/>
-        <v>0.19047619047619047</v>
+        <v>0.2</v>
       </c>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
@@ -3992,9 +4126,11 @@
       <c r="AB36" s="45"/>
       <c r="AC36" s="44"/>
       <c r="AD36" s="45"/>
-      <c r="AE36" s="44"/>
-      <c r="AF36" s="45"/>
-      <c r="AG36" s="44"/>
+      <c r="AE36" s="42"/>
+      <c r="AF36" s="43"/>
+      <c r="AG36" s="44">
+        <v>1</v>
+      </c>
       <c r="AH36" s="45"/>
       <c r="AI36" s="44"/>
       <c r="AJ36" s="45"/>
@@ -4010,7 +4146,7 @@
       </c>
       <c r="D37" s="30">
         <f t="shared" si="5"/>
-        <v>9.5238095238095233E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E37" s="40"/>
       <c r="F37" s="41"/>
@@ -4042,8 +4178,8 @@
       <c r="AB37" s="41"/>
       <c r="AC37" s="40"/>
       <c r="AD37" s="41"/>
-      <c r="AE37" s="40"/>
-      <c r="AF37" s="41"/>
+      <c r="AE37" s="42"/>
+      <c r="AF37" s="43"/>
       <c r="AG37" s="40"/>
       <c r="AH37" s="41"/>
       <c r="AI37" s="40"/>
@@ -4060,7 +4196,7 @@
       </c>
       <c r="D38" s="30">
         <f t="shared" si="5"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="41"/>
@@ -4090,8 +4226,8 @@
       <c r="AB38" s="41"/>
       <c r="AC38" s="40"/>
       <c r="AD38" s="41"/>
-      <c r="AE38" s="40"/>
-      <c r="AF38" s="41"/>
+      <c r="AE38" s="42"/>
+      <c r="AF38" s="43"/>
       <c r="AG38" s="40"/>
       <c r="AH38" s="41"/>
       <c r="AI38" s="40"/>
@@ -4108,7 +4244,7 @@
       </c>
       <c r="D39" s="30">
         <f t="shared" si="5"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E39" s="40"/>
       <c r="F39" s="41"/>
@@ -4138,8 +4274,8 @@
       <c r="AB39" s="41"/>
       <c r="AC39" s="40"/>
       <c r="AD39" s="41"/>
-      <c r="AE39" s="40"/>
-      <c r="AF39" s="41"/>
+      <c r="AE39" s="42"/>
+      <c r="AF39" s="43"/>
       <c r="AG39" s="40"/>
       <c r="AH39" s="41"/>
       <c r="AI39" s="40"/>
@@ -4156,7 +4292,7 @@
       </c>
       <c r="D40" s="30">
         <f t="shared" si="5"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="41"/>
@@ -4186,8 +4322,8 @@
       <c r="AB40" s="41"/>
       <c r="AC40" s="40"/>
       <c r="AD40" s="41"/>
-      <c r="AE40" s="40"/>
-      <c r="AF40" s="41"/>
+      <c r="AE40" s="42"/>
+      <c r="AF40" s="43"/>
       <c r="AG40" s="40"/>
       <c r="AH40" s="41"/>
       <c r="AI40" s="40"/>
@@ -4230,8 +4366,8 @@
       <c r="AB41" s="41"/>
       <c r="AC41" s="40"/>
       <c r="AD41" s="41"/>
-      <c r="AE41" s="40"/>
-      <c r="AF41" s="41"/>
+      <c r="AE41" s="42"/>
+      <c r="AF41" s="43"/>
       <c r="AG41" s="40"/>
       <c r="AH41" s="41"/>
       <c r="AI41" s="40"/>
@@ -4274,8 +4410,8 @@
       <c r="AB42" s="37"/>
       <c r="AC42" s="36"/>
       <c r="AD42" s="37"/>
-      <c r="AE42" s="36"/>
-      <c r="AF42" s="37"/>
+      <c r="AE42" s="38"/>
+      <c r="AF42" s="39"/>
       <c r="AG42" s="36"/>
       <c r="AH42" s="37"/>
       <c r="AI42" s="36"/>

</xml_diff>